<commit_message>
Stream graph fail cause of  data / new interactive stream graph
</commit_message>
<xml_diff>
--- a/GenderGap_Data/gendergap_06_14.xlsx
+++ b/GenderGap_Data/gendergap_06_14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21820" yWindow="11120" windowWidth="26960" windowHeight="16960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20560" yWindow="10960" windowWidth="26960" windowHeight="16960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="gendergap_06_14.csv" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>United States</t>
   </si>
@@ -137,40 +137,13 @@
     <t>score</t>
   </si>
   <si>
-    <t>23/115</t>
-  </si>
-  <si>
     <t>0.00 = inequality, 1.00 = equality</t>
   </si>
   <si>
-    <t>31/128</t>
-  </si>
-  <si>
-    <t>27/130</t>
-  </si>
-  <si>
     <t>gdp(billions$)</t>
   </si>
   <si>
     <t>pop(million)</t>
-  </si>
-  <si>
-    <t>31/134</t>
-  </si>
-  <si>
-    <t>19/134</t>
-  </si>
-  <si>
-    <t>17/135</t>
-  </si>
-  <si>
-    <t>22/135</t>
-  </si>
-  <si>
-    <t>23/136</t>
-  </si>
-  <si>
-    <t>20/142</t>
   </si>
 </sst>
 </file>
@@ -178,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -249,8 +222,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -339,23 +314,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -391,6 +366,7 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -426,6 +402,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,7 +735,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:M35"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -790,10 +767,10 @@
         <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>29</v>
@@ -1860,7 +1837,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
@@ -1892,7 +1869,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1905,10 +1882,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>29</v>
@@ -1936,8 +1913,9 @@
       <c r="A2" s="1">
         <v>2006</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
+      <c r="B2" s="4">
+        <f xml:space="preserve"> 23/115</f>
+        <v>0.2</v>
       </c>
       <c r="C2" s="1">
         <v>298.2</v>
@@ -1971,8 +1949,9 @@
       <c r="A3" s="1">
         <v>2007</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
+      <c r="B3" s="4">
+        <f xml:space="preserve"> 31/128</f>
+        <v>0.2421875</v>
       </c>
       <c r="C3" s="1">
         <v>296.41000000000003</v>
@@ -2006,8 +1985,9 @@
       <c r="A4" s="1">
         <v>2008</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
+      <c r="B4" s="4">
+        <f xml:space="preserve"> 27/130</f>
+        <v>0.2076923076923077</v>
       </c>
       <c r="C4" s="1">
         <v>301.62</v>
@@ -2041,8 +2021,9 @@
       <c r="A5" s="1">
         <v>2009</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
+      <c r="B5" s="4">
+        <f xml:space="preserve"> 31/134</f>
+        <v>0.23134328358208955</v>
       </c>
       <c r="C5" s="1">
         <v>301.62</v>
@@ -2076,8 +2057,9 @@
       <c r="A6" s="1">
         <v>2010</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
+      <c r="B6" s="4">
+        <f xml:space="preserve"> 19/134</f>
+        <v>0.1417910447761194</v>
       </c>
       <c r="C6" s="1">
         <v>304.06</v>
@@ -2111,8 +2093,9 @@
       <c r="A7" s="1">
         <v>2011</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
+      <c r="B7" s="4">
+        <f xml:space="preserve"> 17/135</f>
+        <v>0.12592592592592591</v>
       </c>
       <c r="C7" s="1">
         <v>309.70999999999998</v>
@@ -2146,8 +2129,9 @@
       <c r="A8" s="1">
         <v>2012</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>46</v>
+      <c r="B8" s="4">
+        <f xml:space="preserve"> 22/135</f>
+        <v>0.16296296296296298</v>
       </c>
       <c r="C8" s="1">
         <v>311.58999999999997</v>
@@ -2181,8 +2165,9 @@
       <c r="A9" s="1">
         <v>2013</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
+      <c r="B9" s="4">
+        <f xml:space="preserve"> 23/136</f>
+        <v>0.16911764705882354</v>
       </c>
       <c r="C9" s="1">
         <v>311.58999999999997</v>
@@ -2216,8 +2201,9 @@
       <c r="A10" s="1">
         <v>2014</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
+      <c r="B10" s="4">
+        <f xml:space="preserve"> 20/142</f>
+        <v>0.14084507042253522</v>
       </c>
       <c r="C10" s="1">
         <v>316.63</v>
@@ -2263,7 +2249,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="A1:K10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2276,10 +2262,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>29</v>

</xml_diff>